<commit_message>
updated methodology with t-test
</commit_message>
<xml_diff>
--- a/results tables/results_table_scheme.xlsx
+++ b/results tables/results_table_scheme.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Financial Results Table - Comp" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="53">
   <si>
     <t>Annual Returns</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Significance test: paired, two tailed t test results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing data </t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -562,30 +565,26 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -594,6 +593,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -607,7 +612,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -628,29 +657,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6079,8 +6094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C19" sqref="C1:I1048576"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76:E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6104,37 +6119,37 @@
   <sheetData>
     <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="71" t="s">
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="71" t="s">
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="73"/>
+      <c r="O3" s="103"/>
+      <c r="P3" s="103"/>
+      <c r="Q3" s="103"/>
+      <c r="R3" s="104"/>
     </row>
     <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="78"/>
-      <c r="C4" s="76"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="101"/>
       <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
@@ -6182,7 +6197,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="89" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -6235,7 +6250,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="80"/>
+      <c r="B6" s="90"/>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
@@ -6286,7 +6301,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="80"/>
+      <c r="B7" s="90"/>
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
@@ -6337,7 +6352,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="80"/>
+      <c r="B8" s="90"/>
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
@@ -6388,7 +6403,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="80"/>
+      <c r="B9" s="90"/>
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
@@ -6439,7 +6454,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="80"/>
+      <c r="B10" s="90"/>
       <c r="C10" s="23" t="s">
         <v>34</v>
       </c>
@@ -6505,7 +6520,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="81"/>
+      <c r="B11" s="91"/>
       <c r="C11" s="23" t="s">
         <v>28</v>
       </c>
@@ -6571,7 +6586,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="89" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -6592,19 +6607,19 @@
       <c r="H12" s="15">
         <v>-0.230341620949573</v>
       </c>
-      <c r="I12" s="98">
+      <c r="I12" s="75">
         <v>3.13156199586615E-2</v>
       </c>
-      <c r="J12" s="99">
+      <c r="J12" s="76">
         <v>0.158923200427808</v>
       </c>
-      <c r="K12" s="100">
+      <c r="K12" s="77">
         <v>-0.19930292535681901</v>
       </c>
-      <c r="L12" s="100">
+      <c r="L12" s="77">
         <v>-0.127850763626391</v>
       </c>
-      <c r="M12" s="101">
+      <c r="M12" s="78">
         <v>-0.122477784622696</v>
       </c>
       <c r="N12" s="37">
@@ -6624,7 +6639,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="80"/>
+      <c r="B13" s="90"/>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
@@ -6643,19 +6658,19 @@
       <c r="H13" s="18">
         <v>-0.31188499352231602</v>
       </c>
-      <c r="I13" s="102">
+      <c r="I13" s="79">
         <v>8.1754085874703401E-3</v>
       </c>
-      <c r="J13" s="103">
+      <c r="J13" s="80">
         <v>2.9686797133156001E-2</v>
       </c>
-      <c r="K13" s="103">
+      <c r="K13" s="80">
         <v>-0.10320913792351399</v>
       </c>
-      <c r="L13" s="104">
+      <c r="L13" s="81">
         <v>-0.13891939698282901</v>
       </c>
-      <c r="M13" s="105">
+      <c r="M13" s="82">
         <v>-0.170175390761545</v>
       </c>
       <c r="N13" s="40">
@@ -6675,7 +6690,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="80"/>
+      <c r="B14" s="90"/>
       <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
@@ -6694,19 +6709,19 @@
       <c r="H14" s="18">
         <v>-0.129084618045535</v>
       </c>
-      <c r="I14" s="102">
+      <c r="I14" s="79">
         <v>0.100798792716777</v>
       </c>
-      <c r="J14" s="103">
+      <c r="J14" s="80">
         <v>0.21694315682008999</v>
       </c>
-      <c r="K14" s="103">
+      <c r="K14" s="80">
         <v>-0.117490800820717</v>
       </c>
-      <c r="L14" s="104">
+      <c r="L14" s="81">
         <v>5.0432248000304297E-2</v>
       </c>
-      <c r="M14" s="105">
+      <c r="M14" s="82">
         <v>-6.6647736206958699E-2</v>
       </c>
       <c r="N14" s="40">
@@ -6726,7 +6741,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="80"/>
+      <c r="B15" s="90"/>
       <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
@@ -6745,19 +6760,19 @@
       <c r="H15" s="18">
         <v>8.0013882383444895E-2</v>
       </c>
-      <c r="I15" s="102">
+      <c r="I15" s="79">
         <v>0.346221039105227</v>
       </c>
-      <c r="J15" s="103">
+      <c r="J15" s="80">
         <v>4.5071649422026003E-2</v>
       </c>
-      <c r="K15" s="103">
+      <c r="K15" s="80">
         <v>-0.22820796269291099</v>
       </c>
-      <c r="L15" s="103">
+      <c r="L15" s="80">
         <v>-0.157324120085719</v>
       </c>
-      <c r="M15" s="106">
+      <c r="M15" s="83">
         <v>3.9160396719383997E-2</v>
       </c>
       <c r="N15" s="40">
@@ -6777,7 +6792,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="80"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="22" t="s">
         <v>9</v>
       </c>
@@ -6796,19 +6811,19 @@
       <c r="H16" s="18">
         <v>-0.19485432500445601</v>
       </c>
-      <c r="I16" s="102">
+      <c r="I16" s="79">
         <v>2.78521185042006E-2</v>
       </c>
-      <c r="J16" s="103">
+      <c r="J16" s="80">
         <v>0.333104580082421</v>
       </c>
-      <c r="K16" s="103">
+      <c r="K16" s="80">
         <v>-0.187076033856686</v>
       </c>
-      <c r="L16" s="103">
+      <c r="L16" s="80">
         <v>-0.16091402964760901</v>
       </c>
-      <c r="M16" s="105">
+      <c r="M16" s="82">
         <v>-0.102514245698078</v>
       </c>
       <c r="N16" s="40">
@@ -6828,7 +6843,7 @@
       </c>
     </row>
     <row r="17" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="80"/>
+      <c r="B17" s="90"/>
       <c r="C17" s="23" t="s">
         <v>34</v>
       </c>
@@ -6852,23 +6867,23 @@
         <f t="shared" ref="H17" si="5">_xlfn.STDEV.S(H12:H16)</f>
         <v>0.14811810171656428</v>
       </c>
-      <c r="I17" s="107">
+      <c r="I17" s="84">
         <f t="shared" ref="I17" si="6">_xlfn.STDEV.S(I12:I16)</f>
         <v>0.14048024379740878</v>
       </c>
-      <c r="J17" s="108">
+      <c r="J17" s="85">
         <f t="shared" ref="J17" si="7">_xlfn.STDEV.S(J12:J16)</f>
         <v>0.1258431446977816</v>
       </c>
-      <c r="K17" s="109">
+      <c r="K17" s="86">
         <f t="shared" ref="K17" si="8">_xlfn.STDEV.S(K12:K16)</f>
         <v>5.4114136898476869E-2</v>
       </c>
-      <c r="L17" s="110">
+      <c r="L17" s="87">
         <f t="shared" ref="L17" si="9">_xlfn.STDEV.S(L12:L16)</f>
         <v>8.8991177468047314E-2</v>
       </c>
-      <c r="M17" s="111">
+      <c r="M17" s="88">
         <f t="shared" ref="M17" si="10">_xlfn.STDEV.S(M12:M16)</f>
         <v>7.8609302891303842E-2</v>
       </c>
@@ -6894,7 +6909,7 @@
       </c>
     </row>
     <row r="18" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="81"/>
+      <c r="B18" s="91"/>
       <c r="C18" s="23" t="s">
         <v>28</v>
       </c>
@@ -6918,23 +6933,23 @@
         <f t="shared" si="16"/>
         <v>-0.15723033502768702</v>
       </c>
-      <c r="I18" s="107">
+      <c r="I18" s="84">
         <f t="shared" si="16"/>
         <v>0.10287259577446728</v>
       </c>
-      <c r="J18" s="109">
+      <c r="J18" s="86">
         <f t="shared" si="16"/>
         <v>0.15674587677710022</v>
       </c>
-      <c r="K18" s="110">
+      <c r="K18" s="87">
         <f t="shared" si="16"/>
         <v>-0.16705737213012942</v>
       </c>
-      <c r="L18" s="110">
+      <c r="L18" s="87">
         <f t="shared" si="16"/>
         <v>-0.10691521246844875</v>
       </c>
-      <c r="M18" s="111">
+      <c r="M18" s="88">
         <f t="shared" si="16"/>
         <v>-8.4530952113978736E-2</v>
       </c>
@@ -6960,7 +6975,7 @@
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="89" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -7013,7 +7028,7 @@
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="80"/>
+      <c r="B20" s="90"/>
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
@@ -7064,7 +7079,7 @@
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="80"/>
+      <c r="B21" s="90"/>
       <c r="C21" s="2" t="s">
         <v>6</v>
       </c>
@@ -7115,7 +7130,7 @@
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="80"/>
+      <c r="B22" s="90"/>
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
@@ -7166,7 +7181,7 @@
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B23" s="80"/>
+      <c r="B23" s="90"/>
       <c r="C23" s="22" t="s">
         <v>9</v>
       </c>
@@ -7217,7 +7232,7 @@
       </c>
     </row>
     <row r="24" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="80"/>
+      <c r="B24" s="90"/>
       <c r="C24" s="23" t="s">
         <v>34</v>
       </c>
@@ -7283,7 +7298,7 @@
       </c>
     </row>
     <row r="25" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="81"/>
+      <c r="B25" s="91"/>
       <c r="C25" s="23" t="s">
         <v>28</v>
       </c>
@@ -7359,35 +7374,35 @@
       <c r="R28" s="2"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B29" s="77" t="s">
+      <c r="B29" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="71" t="s">
+      <c r="D29" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="72"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="73"/>
-      <c r="I29" s="71" t="s">
+      <c r="E29" s="103"/>
+      <c r="F29" s="103"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="104"/>
+      <c r="I29" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="J29" s="72"/>
-      <c r="K29" s="72"/>
-      <c r="L29" s="72"/>
-      <c r="M29" s="73"/>
-      <c r="N29" s="74"/>
-      <c r="O29" s="74"/>
-      <c r="P29" s="74"/>
-      <c r="Q29" s="74"/>
-      <c r="R29" s="74"/>
+      <c r="J29" s="103"/>
+      <c r="K29" s="103"/>
+      <c r="L29" s="103"/>
+      <c r="M29" s="104"/>
+      <c r="N29" s="106"/>
+      <c r="O29" s="106"/>
+      <c r="P29" s="106"/>
+      <c r="Q29" s="106"/>
+      <c r="R29" s="106"/>
     </row>
     <row r="30" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="78"/>
-      <c r="C30" s="76"/>
+      <c r="B30" s="99"/>
+      <c r="C30" s="101"/>
       <c r="D30" s="4" t="s">
         <v>1</v>
       </c>
@@ -7425,7 +7440,7 @@
       <c r="R30" s="2"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B31" s="79" t="s">
+      <c r="B31" s="89" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -7468,7 +7483,7 @@
       <c r="R31" s="2"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B32" s="80"/>
+      <c r="B32" s="90"/>
       <c r="C32" s="2" t="s">
         <v>5</v>
       </c>
@@ -7509,7 +7524,7 @@
       <c r="R32" s="2"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B33" s="80"/>
+      <c r="B33" s="90"/>
       <c r="C33" s="2" t="s">
         <v>6</v>
       </c>
@@ -7550,7 +7565,7 @@
       <c r="R33" s="2"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B34" s="80"/>
+      <c r="B34" s="90"/>
       <c r="C34" s="2" t="s">
         <v>8</v>
       </c>
@@ -7591,7 +7606,7 @@
       <c r="R34" s="2"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B35" s="80"/>
+      <c r="B35" s="90"/>
       <c r="C35" s="2" t="s">
         <v>9</v>
       </c>
@@ -7632,7 +7647,7 @@
       <c r="R35" s="2"/>
     </row>
     <row r="36" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="81"/>
+      <c r="B36" s="91"/>
       <c r="C36" s="55" t="s">
         <v>28</v>
       </c>
@@ -7683,7 +7698,7 @@
       <c r="R36" s="2"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B37" s="79" t="s">
+      <c r="B37" s="89" t="s">
         <v>49</v>
       </c>
       <c r="C37" s="7" t="s">
@@ -7726,7 +7741,7 @@
       <c r="R37" s="2"/>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B38" s="80"/>
+      <c r="B38" s="90"/>
       <c r="C38" s="2" t="s">
         <v>5</v>
       </c>
@@ -7767,7 +7782,7 @@
       <c r="R38" s="2"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B39" s="80"/>
+      <c r="B39" s="90"/>
       <c r="C39" s="2" t="s">
         <v>6</v>
       </c>
@@ -7808,7 +7823,7 @@
       <c r="R39" s="2"/>
     </row>
     <row r="40" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B40" s="80"/>
+      <c r="B40" s="90"/>
       <c r="C40" s="2" t="s">
         <v>8</v>
       </c>
@@ -7849,7 +7864,7 @@
       <c r="R40" s="2"/>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B41" s="80"/>
+      <c r="B41" s="90"/>
       <c r="C41" s="2" t="s">
         <v>9</v>
       </c>
@@ -7890,7 +7905,7 @@
       <c r="R41" s="2"/>
     </row>
     <row r="42" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="81"/>
+      <c r="B42" s="91"/>
       <c r="C42" s="55" t="s">
         <v>28</v>
       </c>
@@ -7941,7 +7956,7 @@
       <c r="R42" s="2"/>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B43" s="79" t="s">
+      <c r="B43" s="89" t="s">
         <v>14</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -7984,7 +7999,7 @@
       <c r="R43" s="2"/>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B44" s="80"/>
+      <c r="B44" s="90"/>
       <c r="C44" s="2" t="s">
         <v>5</v>
       </c>
@@ -8025,7 +8040,7 @@
       <c r="R44" s="2"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B45" s="80"/>
+      <c r="B45" s="90"/>
       <c r="C45" s="2" t="s">
         <v>6</v>
       </c>
@@ -8066,7 +8081,7 @@
       <c r="R45" s="2"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B46" s="80"/>
+      <c r="B46" s="90"/>
       <c r="C46" s="2" t="s">
         <v>8</v>
       </c>
@@ -8107,7 +8122,7 @@
       <c r="R46" s="2"/>
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B47" s="80"/>
+      <c r="B47" s="90"/>
       <c r="C47" s="2" t="s">
         <v>9</v>
       </c>
@@ -8148,7 +8163,7 @@
       <c r="R47" s="2"/>
     </row>
     <row r="48" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="81"/>
+      <c r="B48" s="91"/>
       <c r="C48" s="55" t="s">
         <v>28</v>
       </c>
@@ -8216,17 +8231,17 @@
       <c r="R50" s="2"/>
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B51" s="82" t="s">
+      <c r="B51" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="84" t="s">
+      <c r="C51" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="D51" s="85"/>
-      <c r="E51" s="86" t="s">
+      <c r="D51" s="97"/>
+      <c r="E51" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="F51" s="85"/>
+      <c r="F51" s="97"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
@@ -8234,7 +8249,7 @@
       <c r="R51" s="2"/>
     </row>
     <row r="52" spans="2:18" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="83"/>
+      <c r="B52" s="95"/>
       <c r="C52" s="61" t="s">
         <v>36</v>
       </c>
@@ -8258,7 +8273,7 @@
       <c r="R52" s="2"/>
     </row>
     <row r="53" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="79" t="s">
+      <c r="B53" s="89" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -8275,7 +8290,7 @@
       </c>
     </row>
     <row r="54" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B54" s="80"/>
+      <c r="B54" s="90"/>
       <c r="C54" s="1" t="s">
         <v>1</v>
       </c>
@@ -8290,7 +8305,7 @@
       </c>
     </row>
     <row r="55" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="80"/>
+      <c r="B55" s="90"/>
       <c r="C55" s="1" t="s">
         <v>1</v>
       </c>
@@ -8305,7 +8320,7 @@
       </c>
     </row>
     <row r="56" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B56" s="80"/>
+      <c r="B56" s="90"/>
       <c r="C56" s="1" t="s">
         <v>1</v>
       </c>
@@ -8320,7 +8335,7 @@
       </c>
     </row>
     <row r="57" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B57" s="80"/>
+      <c r="B57" s="90"/>
       <c r="C57" s="1" t="s">
         <v>2</v>
       </c>
@@ -8335,7 +8350,7 @@
       </c>
     </row>
     <row r="58" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B58" s="80"/>
+      <c r="B58" s="90"/>
       <c r="C58" s="1" t="s">
         <v>2</v>
       </c>
@@ -8350,7 +8365,7 @@
       </c>
     </row>
     <row r="59" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="81"/>
+      <c r="B59" s="91"/>
       <c r="C59" s="4" t="s">
         <v>2</v>
       </c>
@@ -8365,7 +8380,7 @@
       </c>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B60" s="79" t="s">
+      <c r="B60" s="89" t="s">
         <v>49</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -8382,7 +8397,7 @@
       </c>
     </row>
     <row r="61" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B61" s="80"/>
+      <c r="B61" s="90"/>
       <c r="C61" s="1" t="s">
         <v>1</v>
       </c>
@@ -8397,7 +8412,7 @@
       </c>
     </row>
     <row r="62" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="80"/>
+      <c r="B62" s="90"/>
       <c r="C62" s="1" t="s">
         <v>1</v>
       </c>
@@ -8412,7 +8427,7 @@
       </c>
     </row>
     <row r="63" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B63" s="80"/>
+      <c r="B63" s="90"/>
       <c r="C63" s="1" t="s">
         <v>1</v>
       </c>
@@ -8427,7 +8442,7 @@
       </c>
     </row>
     <row r="64" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B64" s="80"/>
+      <c r="B64" s="90"/>
       <c r="C64" s="1" t="s">
         <v>2</v>
       </c>
@@ -8442,7 +8457,7 @@
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B65" s="80"/>
+      <c r="B65" s="90"/>
       <c r="C65" s="1" t="s">
         <v>2</v>
       </c>
@@ -8457,7 +8472,7 @@
       </c>
     </row>
     <row r="66" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="81"/>
+      <c r="B66" s="91"/>
       <c r="C66" s="4" t="s">
         <v>2</v>
       </c>
@@ -8472,7 +8487,7 @@
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B67" s="79" t="s">
+      <c r="B67" s="89" t="s">
         <v>42</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -8489,7 +8504,7 @@
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B68" s="80"/>
+      <c r="B68" s="90"/>
       <c r="C68" s="1" t="s">
         <v>1</v>
       </c>
@@ -8504,7 +8519,7 @@
       </c>
     </row>
     <row r="69" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="80"/>
+      <c r="B69" s="90"/>
       <c r="C69" s="1" t="s">
         <v>1</v>
       </c>
@@ -8519,7 +8534,7 @@
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B70" s="80"/>
+      <c r="B70" s="90"/>
       <c r="C70" s="1" t="s">
         <v>1</v>
       </c>
@@ -8534,7 +8549,7 @@
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B71" s="80"/>
+      <c r="B71" s="90"/>
       <c r="C71" s="1" t="s">
         <v>2</v>
       </c>
@@ -8549,7 +8564,7 @@
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B72" s="80"/>
+      <c r="B72" s="90"/>
       <c r="C72" s="1" t="s">
         <v>2</v>
       </c>
@@ -8564,7 +8579,7 @@
       </c>
     </row>
     <row r="73" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="81"/>
+      <c r="B73" s="91"/>
       <c r="C73" s="4" t="s">
         <v>2</v>
       </c>
@@ -8584,29 +8599,29 @@
       </c>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B77" s="82" t="s">
+      <c r="B77" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="C77" s="84" t="s">
+      <c r="C77" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="D77" s="85"/>
-      <c r="E77" s="96" t="s">
+      <c r="D77" s="97"/>
+      <c r="E77" s="92" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="78" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="83"/>
+      <c r="B78" s="95"/>
       <c r="C78" s="61" t="s">
         <v>36</v>
       </c>
       <c r="D78" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="E78" s="97"/>
+      <c r="E78" s="93"/>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B79" s="79" t="s">
+      <c r="B79" s="89" t="s">
         <v>13</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -8615,84 +8630,84 @@
       <c r="D79" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E79" s="93">
+      <c r="E79" s="72">
         <v>0.41360538776069</v>
       </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B80" s="80"/>
+      <c r="B80" s="90"/>
       <c r="C80" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E80" s="94">
+      <c r="E80" s="73">
         <v>0.121441303508643</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B81" s="80"/>
+      <c r="B81" s="90"/>
       <c r="C81" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E81" s="94">
+      <c r="E81" s="73">
         <v>0.39032689443521901</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B82" s="80"/>
+      <c r="B82" s="90"/>
       <c r="C82" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E82" s="94">
+      <c r="E82" s="73">
         <v>0.28303301606163001</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B83" s="80"/>
+      <c r="B83" s="90"/>
       <c r="C83" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E83" s="94">
+      <c r="E83" s="73">
         <v>0.91240527820265105</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B84" s="80"/>
+      <c r="B84" s="90"/>
       <c r="C84" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E84" s="94">
+      <c r="E84" s="73">
         <v>0.91561230816444406</v>
       </c>
     </row>
     <row r="85" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="81"/>
+      <c r="B85" s="91"/>
       <c r="C85" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E85" s="95">
+      <c r="E85" s="74">
         <v>0.58281054981942104</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B86" s="79" t="s">
+      <c r="B86" s="89" t="s">
         <v>49</v>
       </c>
       <c r="C86" s="1" t="s">
@@ -8701,84 +8716,84 @@
       <c r="D86" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E86" s="93">
+      <c r="E86" s="72">
         <v>0.61830988814292298</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B87" s="80"/>
+      <c r="B87" s="90"/>
       <c r="C87" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E87" s="94">
+      <c r="E87" s="73">
         <v>2.6950568015114799E-2</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B88" s="80"/>
+      <c r="B88" s="90"/>
       <c r="C88" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E88" s="94">
+      <c r="E88" s="73">
         <v>5.2780005060125597E-2</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B89" s="80"/>
+      <c r="B89" s="90"/>
       <c r="C89" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E89" s="94">
+      <c r="E89" s="73">
         <v>3.76288118769986E-3</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B90" s="80"/>
+      <c r="B90" s="90"/>
       <c r="C90" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E90" s="94">
+      <c r="E90" s="73">
         <v>6.7135643499659E-3</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B91" s="80"/>
+      <c r="B91" s="90"/>
       <c r="C91" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E91" s="94">
+      <c r="E91" s="73">
         <v>1.28266939548603E-2</v>
       </c>
     </row>
     <row r="92" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="81"/>
+      <c r="B92" s="91"/>
       <c r="C92" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E92" s="95">
+      <c r="E92" s="74">
         <v>2.6248695470517801E-2</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B93" s="79" t="s">
+      <c r="B93" s="89" t="s">
         <v>42</v>
       </c>
       <c r="C93" s="1" t="s">
@@ -8787,90 +8802,94 @@
       <c r="D93" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E93" s="93">
+      <c r="E93" s="72">
         <v>0.47830138352062701</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B94" s="80"/>
+      <c r="B94" s="90"/>
       <c r="C94" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E94" s="94">
+      <c r="E94" s="73">
         <v>0.97197132058742897</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B95" s="80"/>
+      <c r="B95" s="90"/>
       <c r="C95" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E95" s="94">
+      <c r="E95" s="73">
         <v>0.85006904973170005</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B96" s="80"/>
+      <c r="B96" s="90"/>
       <c r="C96" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E96" s="94">
+      <c r="E96" s="73">
         <v>0.29653350275301099</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B97" s="80"/>
+      <c r="B97" s="90"/>
       <c r="C97" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E97" s="94">
+      <c r="E97" s="73">
         <v>0.70647571413425103</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B98" s="80"/>
+      <c r="B98" s="90"/>
       <c r="C98" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E98" s="94">
+      <c r="E98" s="73">
         <v>0.95486260717246696</v>
       </c>
     </row>
     <row r="99" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B99" s="81"/>
+      <c r="B99" s="91"/>
       <c r="C99" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E99" s="95">
+      <c r="E99" s="74">
         <v>0.46781233141728401</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B93:B99"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="B79:B85"/>
-    <mergeCell ref="B86:B92"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="N29:R29"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="I3:M3"/>
     <mergeCell ref="B60:B66"/>
     <mergeCell ref="B67:B73"/>
     <mergeCell ref="B29:B30"/>
@@ -8883,16 +8902,12 @@
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="B37:B42"/>
     <mergeCell ref="B43:B48"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="N29:R29"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="B93:B99"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="B79:B85"/>
+    <mergeCell ref="B86:B92"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8902,10 +8917,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:X48"/>
+  <dimension ref="B2:X64"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52:D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8926,46 +8941,46 @@
     </row>
     <row r="3" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="89" t="s">
+      <c r="D4" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="89" t="s">
+      <c r="E4" s="110"/>
+      <c r="F4" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91" t="s">
+      <c r="G4" s="110"/>
+      <c r="H4" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="92"/>
-      <c r="J4" s="91" t="s">
+      <c r="I4" s="112"/>
+      <c r="J4" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="92"/>
-      <c r="P4" s="77" t="s">
+      <c r="K4" s="112"/>
+      <c r="P4" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="75" t="s">
+      <c r="Q4" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="87" t="s">
+      <c r="R4" s="107" t="s">
         <v>32</v>
       </c>
-      <c r="S4" s="88"/>
-      <c r="T4" s="87" t="s">
+      <c r="S4" s="108"/>
+      <c r="T4" s="107" t="s">
         <v>48</v>
       </c>
-      <c r="U4" s="88"/>
+      <c r="U4" s="108"/>
     </row>
     <row r="5" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="78"/>
-      <c r="C5" s="76"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="101"/>
       <c r="D5" s="4" t="s">
         <v>1</v>
       </c>
@@ -8990,8 +9005,8 @@
       <c r="K5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="76"/>
+      <c r="P5" s="99"/>
+      <c r="Q5" s="101"/>
       <c r="R5" s="4" t="s">
         <v>1</v>
       </c>
@@ -9006,7 +9021,7 @@
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="89" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -9036,7 +9051,7 @@
       <c r="K6" s="15">
         <v>0.46449738029316001</v>
       </c>
-      <c r="P6" s="79" t="s">
+      <c r="P6" s="89" t="s">
         <v>13</v>
       </c>
       <c r="Q6" s="7" t="s">
@@ -9061,7 +9076,7 @@
       <c r="X6" s="69"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B7" s="80"/>
+      <c r="B7" s="90"/>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
@@ -9089,7 +9104,7 @@
       <c r="K7" s="18">
         <v>0.54328564517243705</v>
       </c>
-      <c r="P7" s="80"/>
+      <c r="P7" s="90"/>
       <c r="Q7" s="2" t="s">
         <v>5</v>
       </c>
@@ -9112,7 +9127,7 @@
       <c r="X7" s="69"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B8" s="80"/>
+      <c r="B8" s="90"/>
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
@@ -9140,7 +9155,7 @@
       <c r="K8" s="18">
         <v>0.44666666666666599</v>
       </c>
-      <c r="P8" s="80"/>
+      <c r="P8" s="90"/>
       <c r="Q8" s="2" t="s">
         <v>6</v>
       </c>
@@ -9163,7 +9178,7 @@
       <c r="X8" s="69"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B9" s="80"/>
+      <c r="B9" s="90"/>
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
@@ -9191,7 +9206,7 @@
       <c r="K9" s="18">
         <v>0.41017800027812501</v>
       </c>
-      <c r="P9" s="80"/>
+      <c r="P9" s="90"/>
       <c r="Q9" s="2" t="s">
         <v>8</v>
       </c>
@@ -9214,7 +9229,7 @@
       <c r="X9" s="69"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B10" s="80"/>
+      <c r="B10" s="90"/>
       <c r="C10" s="22" t="s">
         <v>9</v>
       </c>
@@ -9242,7 +9257,7 @@
       <c r="K10" s="18">
         <v>0.49500251862456501</v>
       </c>
-      <c r="P10" s="80"/>
+      <c r="P10" s="90"/>
       <c r="Q10" s="22" t="s">
         <v>9</v>
       </c>
@@ -9265,7 +9280,7 @@
       <c r="X10" s="69"/>
     </row>
     <row r="11" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="81"/>
+      <c r="B11" s="91"/>
       <c r="C11" s="24" t="s">
         <v>28</v>
       </c>
@@ -9301,7 +9316,7 @@
         <f t="shared" si="0"/>
         <v>0.47192604220699064</v>
       </c>
-      <c r="P11" s="81"/>
+      <c r="P11" s="91"/>
       <c r="Q11" s="24" t="s">
         <v>28</v>
       </c>
@@ -9326,7 +9341,7 @@
       <c r="X11" s="69"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="89" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -9356,7 +9371,7 @@
       <c r="K12" s="15">
         <v>0.37968877968877901</v>
       </c>
-      <c r="P12" s="79" t="s">
+      <c r="P12" s="89" t="s">
         <v>49</v>
       </c>
       <c r="Q12" s="7" t="s">
@@ -9381,7 +9396,7 @@
       <c r="X12" s="69"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B13" s="80"/>
+      <c r="B13" s="90"/>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
@@ -9409,7 +9424,7 @@
       <c r="K13" s="18">
         <v>0.39484960917629702</v>
       </c>
-      <c r="P13" s="80"/>
+      <c r="P13" s="90"/>
       <c r="Q13" s="2" t="s">
         <v>5</v>
       </c>
@@ -9432,7 +9447,7 @@
       <c r="X13" s="69"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B14" s="80"/>
+      <c r="B14" s="90"/>
       <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
@@ -9460,7 +9475,7 @@
       <c r="K14" s="18">
         <v>0.40748727163821502</v>
       </c>
-      <c r="P14" s="80"/>
+      <c r="P14" s="90"/>
       <c r="Q14" s="2" t="s">
         <v>6</v>
       </c>
@@ -9483,7 +9498,7 @@
       <c r="X14" s="69"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B15" s="80"/>
+      <c r="B15" s="90"/>
       <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
@@ -9511,7 +9526,7 @@
       <c r="K15" s="18">
         <v>0.40951374720683897</v>
       </c>
-      <c r="P15" s="80"/>
+      <c r="P15" s="90"/>
       <c r="Q15" s="2" t="s">
         <v>8</v>
       </c>
@@ -9534,7 +9549,7 @@
       <c r="X15" s="69"/>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B16" s="80"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="22" t="s">
         <v>9</v>
       </c>
@@ -9562,7 +9577,7 @@
       <c r="K16" s="18">
         <v>0.41772262371900498</v>
       </c>
-      <c r="P16" s="80"/>
+      <c r="P16" s="90"/>
       <c r="Q16" s="22" t="s">
         <v>9</v>
       </c>
@@ -9585,7 +9600,7 @@
       <c r="X16" s="69"/>
     </row>
     <row r="17" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="81"/>
+      <c r="B17" s="91"/>
       <c r="C17" s="24" t="s">
         <v>28</v>
       </c>
@@ -9621,7 +9636,7 @@
         <f t="shared" si="1"/>
         <v>0.40185240628582697</v>
       </c>
-      <c r="P17" s="81"/>
+      <c r="P17" s="91"/>
       <c r="Q17" s="24" t="s">
         <v>28</v>
       </c>
@@ -9646,7 +9661,7 @@
       <c r="X17" s="69"/>
     </row>
     <row r="18" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B18" s="79" t="s">
+      <c r="B18" s="89" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -9676,7 +9691,7 @@
       <c r="K18" s="15">
         <v>0.56784646348476098</v>
       </c>
-      <c r="P18" s="79" t="s">
+      <c r="P18" s="89" t="s">
         <v>14</v>
       </c>
       <c r="Q18" s="7" t="s">
@@ -9701,7 +9716,7 @@
       <c r="X18" s="69"/>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B19" s="80"/>
+      <c r="B19" s="90"/>
       <c r="C19" s="2" t="s">
         <v>5</v>
       </c>
@@ -9729,7 +9744,7 @@
       <c r="K19" s="18">
         <v>0.46253496058987997</v>
       </c>
-      <c r="P19" s="80"/>
+      <c r="P19" s="90"/>
       <c r="Q19" s="2" t="s">
         <v>5</v>
       </c>
@@ -9752,7 +9767,7 @@
       <c r="X19" s="69"/>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B20" s="80"/>
+      <c r="B20" s="90"/>
       <c r="C20" s="2" t="s">
         <v>6</v>
       </c>
@@ -9780,7 +9795,7 @@
       <c r="K20" s="18">
         <v>0.50257522316750003</v>
       </c>
-      <c r="P20" s="80"/>
+      <c r="P20" s="90"/>
       <c r="Q20" s="2" t="s">
         <v>6</v>
       </c>
@@ -9803,7 +9818,7 @@
       <c r="X20" s="69"/>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B21" s="80"/>
+      <c r="B21" s="90"/>
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
@@ -9831,7 +9846,7 @@
       <c r="K21" s="18">
         <v>0.49256491545893699</v>
       </c>
-      <c r="P21" s="80"/>
+      <c r="P21" s="90"/>
       <c r="Q21" s="2" t="s">
         <v>8</v>
       </c>
@@ -9854,7 +9869,7 @@
       <c r="X21" s="69"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B22" s="80"/>
+      <c r="B22" s="90"/>
       <c r="C22" s="22" t="s">
         <v>9</v>
       </c>
@@ -9882,7 +9897,7 @@
       <c r="K22" s="18">
         <v>0.53429525850500204</v>
       </c>
-      <c r="P22" s="80"/>
+      <c r="P22" s="90"/>
       <c r="Q22" s="22" t="s">
         <v>9</v>
       </c>
@@ -9905,7 +9920,7 @@
       <c r="X22" s="69"/>
     </row>
     <row r="23" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="81"/>
+      <c r="B23" s="91"/>
       <c r="C23" s="24" t="s">
         <v>28</v>
       </c>
@@ -9941,7 +9956,7 @@
         <f t="shared" si="3"/>
         <v>0.51196336424121602</v>
       </c>
-      <c r="P23" s="81"/>
+      <c r="P23" s="91"/>
       <c r="Q23" s="24" t="s">
         <v>28</v>
       </c>
@@ -10020,7 +10035,7 @@
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="79" t="s">
+      <c r="B37" s="89" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="8" t="s">
@@ -10031,7 +10046,7 @@
       </c>
     </row>
     <row r="38" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="80"/>
+      <c r="B38" s="90"/>
       <c r="C38" s="1" t="s">
         <v>45</v>
       </c>
@@ -10040,7 +10055,7 @@
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="80"/>
+      <c r="B39" s="90"/>
       <c r="C39" s="1" t="s">
         <v>46</v>
       </c>
@@ -10049,7 +10064,7 @@
       </c>
     </row>
     <row r="40" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="81"/>
+      <c r="B40" s="91"/>
       <c r="C40" s="4" t="s">
         <v>47</v>
       </c>
@@ -10058,7 +10073,7 @@
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="79" t="s">
+      <c r="B41" s="89" t="s">
         <v>49</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -10069,7 +10084,7 @@
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="80"/>
+      <c r="B42" s="90"/>
       <c r="C42" s="1" t="s">
         <v>45</v>
       </c>
@@ -10078,7 +10093,7 @@
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="80"/>
+      <c r="B43" s="90"/>
       <c r="C43" s="1" t="s">
         <v>46</v>
       </c>
@@ -10087,7 +10102,7 @@
       </c>
     </row>
     <row r="44" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="81"/>
+      <c r="B44" s="91"/>
       <c r="C44" s="4" t="s">
         <v>47</v>
       </c>
@@ -10096,7 +10111,7 @@
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="79" t="s">
+      <c r="B45" s="89" t="s">
         <v>42</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -10107,7 +10122,7 @@
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="80"/>
+      <c r="B46" s="90"/>
       <c r="C46" s="1" t="s">
         <v>45</v>
       </c>
@@ -10116,7 +10131,7 @@
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="80"/>
+      <c r="B47" s="90"/>
       <c r="C47" s="1" t="s">
         <v>46</v>
       </c>
@@ -10125,7 +10140,7 @@
       </c>
     </row>
     <row r="48" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="81"/>
+      <c r="B48" s="91"/>
       <c r="C48" s="4" t="s">
         <v>47</v>
       </c>
@@ -10133,13 +10148,141 @@
         <v>0</v>
       </c>
     </row>
+    <row r="51" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B51" s="60" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="119" t="s">
+        <v>44</v>
+      </c>
+      <c r="D52" s="71" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B53" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="113" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="116">
+        <v>3.2270088011799301E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B54" s="90"/>
+      <c r="C54" s="114" t="s">
+        <v>45</v>
+      </c>
+      <c r="D54" s="117">
+        <v>2.2265568353040601E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B55" s="90"/>
+      <c r="C55" s="114" t="s">
+        <v>46</v>
+      </c>
+      <c r="D55" s="117">
+        <v>1.6712920535199101E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="91"/>
+      <c r="C56" s="115" t="s">
+        <v>47</v>
+      </c>
+      <c r="D56" s="118">
+        <v>3.1726306288855201E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B57" s="89" t="s">
+        <v>49</v>
+      </c>
+      <c r="C57" s="113" t="s">
+        <v>20</v>
+      </c>
+      <c r="D57" s="116">
+        <v>7.7688539348127404E-5</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B58" s="90"/>
+      <c r="C58" s="114" t="s">
+        <v>45</v>
+      </c>
+      <c r="D58" s="117">
+        <v>1.68102373681875E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B59" s="90"/>
+      <c r="C59" s="114" t="s">
+        <v>46</v>
+      </c>
+      <c r="D59" s="117">
+        <v>1.6282915528986901E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="91"/>
+      <c r="C60" s="115" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60" s="118">
+        <v>1.8619781158812101E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B61" s="89" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" s="113" t="s">
+        <v>20</v>
+      </c>
+      <c r="D61" s="116">
+        <v>1.3627117562528099E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B62" s="90"/>
+      <c r="C62" s="114" t="s">
+        <v>45</v>
+      </c>
+      <c r="D62" s="117">
+        <v>2.9965139606230899E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B63" s="90"/>
+      <c r="C63" s="114" t="s">
+        <v>46</v>
+      </c>
+      <c r="D63" s="117">
+        <v>2.0897722453687298E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="91"/>
+      <c r="C64" s="115" t="s">
+        <v>47</v>
+      </c>
+      <c r="D64" s="118">
+        <v>4.0639486365357004E-3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="P6:P11"/>
-    <mergeCell ref="P12:P17"/>
-    <mergeCell ref="P18:P23"/>
-    <mergeCell ref="B37:B40"/>
+  <mergeCells count="22">
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B53:B56"/>
     <mergeCell ref="B41:B44"/>
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="T4:U4"/>
@@ -10154,6 +10297,11 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B6:B11"/>
     <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="P6:P11"/>
+    <mergeCell ref="P12:P17"/>
+    <mergeCell ref="P18:P23"/>
+    <mergeCell ref="B37:B40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
almost  final clean up
</commit_message>
<xml_diff>
--- a/results tables/results_table_scheme.xlsx
+++ b/results tables/results_table_scheme.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23148" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23148" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Financial Results Table - Comp" sheetId="1" r:id="rId1"/>
@@ -625,6 +625,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -633,12 +657,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -652,32 +670,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -14424,8 +14424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:M9"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37:M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14437,10 +14437,11 @@
     <col min="6" max="6" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
     <col min="8" max="8" width="8.5546875" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="7" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.5546875" bestFit="1" customWidth="1"/>
@@ -14449,37 +14450,37 @@
   <sheetData>
     <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="112" t="s">
+      <c r="C3" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="114" t="s">
+      <c r="D3" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="114" t="s">
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="115"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="114" t="s">
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="115"/>
-      <c r="P3" s="115"/>
-      <c r="Q3" s="115"/>
-      <c r="R3" s="116"/>
+      <c r="O3" s="102"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="102"/>
+      <c r="R3" s="103"/>
     </row>
     <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="111"/>
-      <c r="C4" s="113"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="106"/>
       <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
@@ -14527,7 +14528,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="109" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -14580,7 +14581,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="102"/>
+      <c r="B6" s="110"/>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
@@ -14631,7 +14632,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="102"/>
+      <c r="B7" s="110"/>
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
@@ -14682,7 +14683,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="102"/>
+      <c r="B8" s="110"/>
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
@@ -14733,7 +14734,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="102"/>
+      <c r="B9" s="110"/>
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
@@ -14784,7 +14785,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="102"/>
+      <c r="B10" s="110"/>
       <c r="C10" s="23" t="s">
         <v>34</v>
       </c>
@@ -14850,7 +14851,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="103"/>
+      <c r="B11" s="111"/>
       <c r="C11" s="23" t="s">
         <v>28</v>
       </c>
@@ -14916,7 +14917,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="101" t="s">
+      <c r="B12" s="109" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -14969,7 +14970,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="102"/>
+      <c r="B13" s="110"/>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
@@ -15020,7 +15021,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="102"/>
+      <c r="B14" s="110"/>
       <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
@@ -15071,7 +15072,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="102"/>
+      <c r="B15" s="110"/>
       <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
@@ -15122,7 +15123,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="102"/>
+      <c r="B16" s="110"/>
       <c r="C16" s="22" t="s">
         <v>9</v>
       </c>
@@ -15173,7 +15174,7 @@
       </c>
     </row>
     <row r="17" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="102"/>
+      <c r="B17" s="110"/>
       <c r="C17" s="23" t="s">
         <v>34</v>
       </c>
@@ -15239,7 +15240,7 @@
       </c>
     </row>
     <row r="18" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="103"/>
+      <c r="B18" s="111"/>
       <c r="C18" s="23" t="s">
         <v>28</v>
       </c>
@@ -15305,7 +15306,7 @@
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19" s="101" t="s">
+      <c r="B19" s="109" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -15358,7 +15359,7 @@
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="102"/>
+      <c r="B20" s="110"/>
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
@@ -15409,7 +15410,7 @@
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="102"/>
+      <c r="B21" s="110"/>
       <c r="C21" s="2" t="s">
         <v>6</v>
       </c>
@@ -15460,7 +15461,7 @@
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="102"/>
+      <c r="B22" s="110"/>
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
@@ -15511,7 +15512,7 @@
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B23" s="102"/>
+      <c r="B23" s="110"/>
       <c r="C23" s="22" t="s">
         <v>9</v>
       </c>
@@ -15562,7 +15563,7 @@
       </c>
     </row>
     <row r="24" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="102"/>
+      <c r="B24" s="110"/>
       <c r="C24" s="23" t="s">
         <v>34</v>
       </c>
@@ -15628,7 +15629,7 @@
       </c>
     </row>
     <row r="25" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="103"/>
+      <c r="B25" s="111"/>
       <c r="C25" s="23" t="s">
         <v>28</v>
       </c>
@@ -15704,35 +15705,35 @@
       <c r="R28" s="2"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B29" s="110" t="s">
+      <c r="B29" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="112" t="s">
+      <c r="C29" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="114" t="s">
+      <c r="D29" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="115"/>
-      <c r="F29" s="115"/>
-      <c r="G29" s="115"/>
-      <c r="H29" s="116"/>
-      <c r="I29" s="114" t="s">
+      <c r="E29" s="102"/>
+      <c r="F29" s="102"/>
+      <c r="G29" s="102"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="J29" s="115"/>
-      <c r="K29" s="115"/>
-      <c r="L29" s="115"/>
-      <c r="M29" s="116"/>
-      <c r="N29" s="118"/>
-      <c r="O29" s="118"/>
-      <c r="P29" s="118"/>
-      <c r="Q29" s="118"/>
-      <c r="R29" s="118"/>
+      <c r="J29" s="102"/>
+      <c r="K29" s="102"/>
+      <c r="L29" s="102"/>
+      <c r="M29" s="103"/>
+      <c r="N29" s="104"/>
+      <c r="O29" s="104"/>
+      <c r="P29" s="104"/>
+      <c r="Q29" s="104"/>
+      <c r="R29" s="104"/>
     </row>
     <row r="30" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="111"/>
-      <c r="C30" s="113"/>
+      <c r="B30" s="108"/>
+      <c r="C30" s="106"/>
       <c r="D30" s="4" t="s">
         <v>1</v>
       </c>
@@ -15770,7 +15771,7 @@
       <c r="R30" s="2"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B31" s="101" t="s">
+      <c r="B31" s="109" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -15813,7 +15814,7 @@
       <c r="R31" s="2"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B32" s="102"/>
+      <c r="B32" s="110"/>
       <c r="C32" s="2" t="s">
         <v>5</v>
       </c>
@@ -15854,7 +15855,7 @@
       <c r="R32" s="2"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B33" s="102"/>
+      <c r="B33" s="110"/>
       <c r="C33" s="2" t="s">
         <v>6</v>
       </c>
@@ -15895,7 +15896,7 @@
       <c r="R33" s="2"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B34" s="102"/>
+      <c r="B34" s="110"/>
       <c r="C34" s="2" t="s">
         <v>8</v>
       </c>
@@ -15936,7 +15937,7 @@
       <c r="R34" s="2"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B35" s="102"/>
+      <c r="B35" s="110"/>
       <c r="C35" s="2" t="s">
         <v>9</v>
       </c>
@@ -15977,7 +15978,7 @@
       <c r="R35" s="2"/>
     </row>
     <row r="36" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="103"/>
+      <c r="B36" s="111"/>
       <c r="C36" s="55" t="s">
         <v>28</v>
       </c>
@@ -16028,40 +16029,40 @@
       <c r="R36" s="2"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B37" s="101" t="s">
+      <c r="B37" s="109" t="s">
         <v>49</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="31">
         <v>637.38056911135197</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="32">
         <v>3438.6510834068099</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="32">
         <v>-3594.3204686532799</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="32">
         <v>-2397.5580472474198</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37" s="33">
         <v>-2303.4162094957301</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I37" s="31">
         <v>11.1821152475675</v>
       </c>
-      <c r="J37" s="7">
+      <c r="J37" s="32">
         <v>53.728923178231497</v>
       </c>
-      <c r="K37" s="7">
+      <c r="K37" s="32">
         <v>-1797.16023432664</v>
       </c>
-      <c r="L37" s="7">
+      <c r="L37" s="32">
         <v>-399.59300787457101</v>
       </c>
-      <c r="M37" s="9">
+      <c r="M37" s="33">
         <v>-1151.70810474786</v>
       </c>
       <c r="N37" s="2"/>
@@ -16071,38 +16072,38 @@
       <c r="R37" s="2"/>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B38" s="102"/>
+      <c r="B38" s="110"/>
       <c r="C38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="34">
         <v>164.49485157052101</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="35">
         <v>603.74204644858003</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38" s="35">
         <v>-1961.0303020301899</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38" s="35">
         <v>-2589.6660337052199</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="36">
         <v>-3118.8499352231602</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I38" s="34">
         <v>3.57597503414177</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="35">
         <v>9.1476067643724299</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="35">
         <v>-245.12878775377399</v>
       </c>
-      <c r="L38" s="2">
+      <c r="L38" s="35">
         <v>-287.74067041169099</v>
       </c>
-      <c r="M38" s="3">
+      <c r="M38" s="36">
         <v>-1559.4249676115801</v>
       </c>
       <c r="N38" s="2"/>
@@ -16112,38 +16113,38 @@
       <c r="R38" s="2"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B39" s="102"/>
+      <c r="B39" s="110"/>
       <c r="C39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="34">
         <v>2122.0565125930498</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="35">
         <v>4820.69426876745</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="35">
         <v>-2215.51815539878</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="35">
         <v>1036.16733526588</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="36">
         <v>-1290.8461804553499</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I39" s="34">
         <v>62.413426840972001</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="35">
         <v>70.892562775992005</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K39" s="35">
         <v>-553.87953884969704</v>
       </c>
-      <c r="L39" s="2">
+      <c r="L39" s="35">
         <v>74.011952518991507</v>
       </c>
-      <c r="M39" s="3">
+      <c r="M39" s="36">
         <v>-645.42309022767597</v>
       </c>
       <c r="N39" s="2"/>
@@ -16153,38 +16154,38 @@
       <c r="R39" s="2"/>
     </row>
     <row r="40" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B40" s="102"/>
+      <c r="B40" s="110"/>
       <c r="C40" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="34">
         <v>8143.8458943412197</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="35">
         <v>923.59956635554704</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="35">
         <v>-4049.3021952571198</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="35">
         <v>-2903.6470875703499</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="36">
         <v>800.138823834449</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I40" s="34">
         <v>271.46152981137402</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="35">
         <v>14.896767199283</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40" s="35">
         <v>-674.88369920952005</v>
       </c>
-      <c r="L40" s="2">
+      <c r="L40" s="35">
         <v>-290.36470875703498</v>
       </c>
-      <c r="M40" s="3">
+      <c r="M40" s="36">
         <v>400.06941191722399</v>
       </c>
       <c r="N40" s="2"/>
@@ -16194,38 +16195,38 @@
       <c r="R40" s="2"/>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B41" s="102"/>
+      <c r="B41" s="110"/>
       <c r="C41" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="34">
         <v>565.91609878907502</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="35">
         <v>7791.3411762679698</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="35">
         <v>-3396.8084938245402</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="35">
         <v>-2964.0966139656098</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="36">
         <v>-1948.54325004456</v>
       </c>
-      <c r="I41" s="1">
+      <c r="I41" s="34">
         <v>15.295029697002001</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="35">
         <v>99.888989439333002</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K41" s="35">
         <v>-1698.4042469122701</v>
       </c>
-      <c r="L41" s="2">
+      <c r="L41" s="35">
         <v>-494.01610232760299</v>
       </c>
-      <c r="M41" s="3">
+      <c r="M41" s="36">
         <v>-974.27162502227998</v>
       </c>
       <c r="N41" s="2"/>
@@ -16235,7 +16236,7 @@
       <c r="R41" s="2"/>
     </row>
     <row r="42" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="103"/>
+      <c r="B42" s="111"/>
       <c r="C42" s="55" t="s">
         <v>28</v>
       </c>
@@ -16286,7 +16287,7 @@
       <c r="R42" s="2"/>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B43" s="101" t="s">
+      <c r="B43" s="109" t="s">
         <v>14</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -16329,7 +16330,7 @@
       <c r="R43" s="2"/>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B44" s="102"/>
+      <c r="B44" s="110"/>
       <c r="C44" s="2" t="s">
         <v>5</v>
       </c>
@@ -16370,7 +16371,7 @@
       <c r="R44" s="2"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B45" s="102"/>
+      <c r="B45" s="110"/>
       <c r="C45" s="2" t="s">
         <v>6</v>
       </c>
@@ -16411,7 +16412,7 @@
       <c r="R45" s="2"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B46" s="102"/>
+      <c r="B46" s="110"/>
       <c r="C46" s="2" t="s">
         <v>8</v>
       </c>
@@ -16452,7 +16453,7 @@
       <c r="R46" s="2"/>
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B47" s="102"/>
+      <c r="B47" s="110"/>
       <c r="C47" s="2" t="s">
         <v>9</v>
       </c>
@@ -16493,7 +16494,7 @@
       <c r="R47" s="2"/>
     </row>
     <row r="48" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="103"/>
+      <c r="B48" s="111"/>
       <c r="C48" s="55" t="s">
         <v>28</v>
       </c>
@@ -16561,17 +16562,17 @@
       <c r="R50" s="2"/>
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B51" s="106" t="s">
+      <c r="B51" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="108" t="s">
+      <c r="C51" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="D51" s="109"/>
-      <c r="E51" s="117" t="s">
+      <c r="D51" s="115"/>
+      <c r="E51" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="F51" s="109"/>
+      <c r="F51" s="115"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
@@ -16579,7 +16580,7 @@
       <c r="R51" s="2"/>
     </row>
     <row r="52" spans="2:18" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="107"/>
+      <c r="B52" s="113"/>
       <c r="C52" s="61" t="s">
         <v>36</v>
       </c>
@@ -16603,7 +16604,7 @@
       <c r="R52" s="2"/>
     </row>
     <row r="53" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="101" t="s">
+      <c r="B53" s="109" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -16620,7 +16621,7 @@
       </c>
     </row>
     <row r="54" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B54" s="102"/>
+      <c r="B54" s="110"/>
       <c r="C54" s="1" t="s">
         <v>1</v>
       </c>
@@ -16635,7 +16636,7 @@
       </c>
     </row>
     <row r="55" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="102"/>
+      <c r="B55" s="110"/>
       <c r="C55" s="1" t="s">
         <v>1</v>
       </c>
@@ -16650,7 +16651,7 @@
       </c>
     </row>
     <row r="56" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B56" s="102"/>
+      <c r="B56" s="110"/>
       <c r="C56" s="1" t="s">
         <v>1</v>
       </c>
@@ -16665,7 +16666,7 @@
       </c>
     </row>
     <row r="57" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B57" s="102"/>
+      <c r="B57" s="110"/>
       <c r="C57" s="1" t="s">
         <v>2</v>
       </c>
@@ -16680,7 +16681,7 @@
       </c>
     </row>
     <row r="58" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B58" s="102"/>
+      <c r="B58" s="110"/>
       <c r="C58" s="1" t="s">
         <v>2</v>
       </c>
@@ -16695,7 +16696,7 @@
       </c>
     </row>
     <row r="59" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="103"/>
+      <c r="B59" s="111"/>
       <c r="C59" s="4" t="s">
         <v>2</v>
       </c>
@@ -16710,7 +16711,7 @@
       </c>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B60" s="101" t="s">
+      <c r="B60" s="109" t="s">
         <v>49</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -16727,7 +16728,7 @@
       </c>
     </row>
     <row r="61" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B61" s="102"/>
+      <c r="B61" s="110"/>
       <c r="C61" s="1" t="s">
         <v>1</v>
       </c>
@@ -16742,7 +16743,7 @@
       </c>
     </row>
     <row r="62" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="102"/>
+      <c r="B62" s="110"/>
       <c r="C62" s="1" t="s">
         <v>1</v>
       </c>
@@ -16757,7 +16758,7 @@
       </c>
     </row>
     <row r="63" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B63" s="102"/>
+      <c r="B63" s="110"/>
       <c r="C63" s="1" t="s">
         <v>1</v>
       </c>
@@ -16772,7 +16773,7 @@
       </c>
     </row>
     <row r="64" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B64" s="102"/>
+      <c r="B64" s="110"/>
       <c r="C64" s="1" t="s">
         <v>2</v>
       </c>
@@ -16787,7 +16788,7 @@
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B65" s="102"/>
+      <c r="B65" s="110"/>
       <c r="C65" s="1" t="s">
         <v>2</v>
       </c>
@@ -16802,7 +16803,7 @@
       </c>
     </row>
     <row r="66" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="103"/>
+      <c r="B66" s="111"/>
       <c r="C66" s="4" t="s">
         <v>2</v>
       </c>
@@ -16817,7 +16818,7 @@
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B67" s="101" t="s">
+      <c r="B67" s="109" t="s">
         <v>42</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -16834,7 +16835,7 @@
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B68" s="102"/>
+      <c r="B68" s="110"/>
       <c r="C68" s="1" t="s">
         <v>1</v>
       </c>
@@ -16849,7 +16850,7 @@
       </c>
     </row>
     <row r="69" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="102"/>
+      <c r="B69" s="110"/>
       <c r="C69" s="1" t="s">
         <v>1</v>
       </c>
@@ -16864,7 +16865,7 @@
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B70" s="102"/>
+      <c r="B70" s="110"/>
       <c r="C70" s="1" t="s">
         <v>1</v>
       </c>
@@ -16879,7 +16880,7 @@
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B71" s="102"/>
+      <c r="B71" s="110"/>
       <c r="C71" s="1" t="s">
         <v>2</v>
       </c>
@@ -16894,7 +16895,7 @@
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B72" s="102"/>
+      <c r="B72" s="110"/>
       <c r="C72" s="1" t="s">
         <v>2</v>
       </c>
@@ -16909,7 +16910,7 @@
       </c>
     </row>
     <row r="73" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="103"/>
+      <c r="B73" s="111"/>
       <c r="C73" s="4" t="s">
         <v>2</v>
       </c>
@@ -16929,29 +16930,29 @@
       </c>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B77" s="106" t="s">
+      <c r="B77" s="112" t="s">
         <v>53</v>
       </c>
-      <c r="C77" s="108" t="s">
+      <c r="C77" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="D77" s="109"/>
-      <c r="E77" s="104" t="s">
+      <c r="D77" s="115"/>
+      <c r="E77" s="117" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="78" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="107"/>
+      <c r="B78" s="113"/>
       <c r="C78" s="61" t="s">
         <v>36</v>
       </c>
       <c r="D78" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="E78" s="105"/>
+      <c r="E78" s="118"/>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B79" s="101" t="s">
+      <c r="B79" s="109" t="s">
         <v>13</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -16965,7 +16966,7 @@
       </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B80" s="102"/>
+      <c r="B80" s="110"/>
       <c r="C80" s="1" t="s">
         <v>1</v>
       </c>
@@ -16977,7 +16978,7 @@
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B81" s="102"/>
+      <c r="B81" s="110"/>
       <c r="C81" s="1" t="s">
         <v>1</v>
       </c>
@@ -16989,7 +16990,7 @@
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B82" s="102"/>
+      <c r="B82" s="110"/>
       <c r="C82" s="1" t="s">
         <v>1</v>
       </c>
@@ -17001,7 +17002,7 @@
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B83" s="102"/>
+      <c r="B83" s="110"/>
       <c r="C83" s="1" t="s">
         <v>2</v>
       </c>
@@ -17013,7 +17014,7 @@
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B84" s="102"/>
+      <c r="B84" s="110"/>
       <c r="C84" s="1" t="s">
         <v>2</v>
       </c>
@@ -17025,7 +17026,7 @@
       </c>
     </row>
     <row r="85" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="103"/>
+      <c r="B85" s="111"/>
       <c r="C85" s="4" t="s">
         <v>2</v>
       </c>
@@ -17037,7 +17038,7 @@
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B86" s="101" t="s">
+      <c r="B86" s="109" t="s">
         <v>49</v>
       </c>
       <c r="C86" s="1" t="s">
@@ -17051,7 +17052,7 @@
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B87" s="102"/>
+      <c r="B87" s="110"/>
       <c r="C87" s="1" t="s">
         <v>1</v>
       </c>
@@ -17063,7 +17064,7 @@
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B88" s="102"/>
+      <c r="B88" s="110"/>
       <c r="C88" s="1" t="s">
         <v>1</v>
       </c>
@@ -17075,7 +17076,7 @@
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B89" s="102"/>
+      <c r="B89" s="110"/>
       <c r="C89" s="1" t="s">
         <v>1</v>
       </c>
@@ -17087,7 +17088,7 @@
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B90" s="102"/>
+      <c r="B90" s="110"/>
       <c r="C90" s="1" t="s">
         <v>2</v>
       </c>
@@ -17099,7 +17100,7 @@
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B91" s="102"/>
+      <c r="B91" s="110"/>
       <c r="C91" s="1" t="s">
         <v>2</v>
       </c>
@@ -17111,7 +17112,7 @@
       </c>
     </row>
     <row r="92" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="103"/>
+      <c r="B92" s="111"/>
       <c r="C92" s="4" t="s">
         <v>2</v>
       </c>
@@ -17123,7 +17124,7 @@
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B93" s="101" t="s">
+      <c r="B93" s="109" t="s">
         <v>42</v>
       </c>
       <c r="C93" s="1" t="s">
@@ -17137,7 +17138,7 @@
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B94" s="102"/>
+      <c r="B94" s="110"/>
       <c r="C94" s="1" t="s">
         <v>1</v>
       </c>
@@ -17149,7 +17150,7 @@
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B95" s="102"/>
+      <c r="B95" s="110"/>
       <c r="C95" s="1" t="s">
         <v>1</v>
       </c>
@@ -17161,7 +17162,7 @@
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B96" s="102"/>
+      <c r="B96" s="110"/>
       <c r="C96" s="1" t="s">
         <v>1</v>
       </c>
@@ -17173,7 +17174,7 @@
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B97" s="102"/>
+      <c r="B97" s="110"/>
       <c r="C97" s="1" t="s">
         <v>2</v>
       </c>
@@ -17185,7 +17186,7 @@
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B98" s="102"/>
+      <c r="B98" s="110"/>
       <c r="C98" s="1" t="s">
         <v>2</v>
       </c>
@@ -17197,7 +17198,7 @@
       </c>
     </row>
     <row r="99" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B99" s="103"/>
+      <c r="B99" s="111"/>
       <c r="C99" s="4" t="s">
         <v>2</v>
       </c>
@@ -17210,16 +17211,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="N29:R29"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="B93:B99"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="B79:B85"/>
+    <mergeCell ref="B86:B92"/>
     <mergeCell ref="B60:B66"/>
     <mergeCell ref="B67:B73"/>
     <mergeCell ref="B29:B30"/>
@@ -17232,12 +17229,16 @@
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="B37:B42"/>
     <mergeCell ref="B43:B48"/>
-    <mergeCell ref="B93:B99"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="B79:B85"/>
-    <mergeCell ref="B86:B92"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="N29:R29"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="I3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17249,7 +17250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="79" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="79" workbookViewId="0">
       <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
@@ -17263,30 +17264,30 @@
       <c r="C2" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="114" t="s">
+      <c r="D2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="114" t="s">
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="115"/>
-      <c r="K2" s="115"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="116"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="103"/>
       <c r="O2" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="114" t="s">
+      <c r="P2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="115"/>
-      <c r="R2" s="115"/>
-      <c r="S2" s="115"/>
-      <c r="T2" s="116"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="102"/>
+      <c r="T2" s="103"/>
     </row>
     <row r="3" spans="1:29" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="99" t="s">
@@ -17345,7 +17346,7 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="109" t="s">
         <v>49</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -17404,7 +17405,7 @@
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B5" s="102"/>
+      <c r="B5" s="110"/>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
@@ -17458,7 +17459,7 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B6" s="102"/>
+      <c r="B6" s="110"/>
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
@@ -17512,7 +17513,7 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B7" s="102"/>
+      <c r="B7" s="110"/>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -17566,7 +17567,7 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="102"/>
+      <c r="B8" s="110"/>
       <c r="C8" s="22" t="s">
         <v>9</v>
       </c>
@@ -17620,7 +17621,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="109" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -17658,7 +17659,7 @@
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B10" s="102"/>
+      <c r="B10" s="110"/>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
@@ -17694,7 +17695,7 @@
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B11" s="102"/>
+      <c r="B11" s="110"/>
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
@@ -17730,7 +17731,7 @@
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B12" s="102"/>
+      <c r="B12" s="110"/>
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
@@ -17766,7 +17767,7 @@
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B13" s="102"/>
+      <c r="B13" s="110"/>
       <c r="C13" s="22" t="s">
         <v>9</v>
       </c>
@@ -19678,10 +19679,10 @@
     </row>
     <row r="3" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="110" t="s">
+      <c r="B4" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="112" t="s">
+      <c r="C4" s="105" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="121" t="s">
@@ -19700,10 +19701,10 @@
         <v>31</v>
       </c>
       <c r="K4" s="124"/>
-      <c r="P4" s="110" t="s">
+      <c r="P4" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="112" t="s">
+      <c r="Q4" s="105" t="s">
         <v>10</v>
       </c>
       <c r="R4" s="119" t="s">
@@ -19716,8 +19717,8 @@
       <c r="U4" s="120"/>
     </row>
     <row r="5" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="111"/>
-      <c r="C5" s="113"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="106"/>
       <c r="D5" s="4" t="s">
         <v>1</v>
       </c>
@@ -19742,8 +19743,8 @@
       <c r="K5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="111"/>
-      <c r="Q5" s="113"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="106"/>
       <c r="R5" s="4" t="s">
         <v>1</v>
       </c>
@@ -19758,7 +19759,7 @@
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B6" s="101" t="s">
+      <c r="B6" s="109" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -19788,7 +19789,7 @@
       <c r="K6" s="15">
         <v>0.46449738029316001</v>
       </c>
-      <c r="P6" s="101" t="s">
+      <c r="P6" s="109" t="s">
         <v>13</v>
       </c>
       <c r="Q6" s="7" t="s">
@@ -19813,7 +19814,7 @@
       <c r="X6" s="69"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B7" s="102"/>
+      <c r="B7" s="110"/>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
@@ -19841,7 +19842,7 @@
       <c r="K7" s="18">
         <v>0.54328564517243705</v>
       </c>
-      <c r="P7" s="102"/>
+      <c r="P7" s="110"/>
       <c r="Q7" s="2" t="s">
         <v>5</v>
       </c>
@@ -19864,7 +19865,7 @@
       <c r="X7" s="69"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B8" s="102"/>
+      <c r="B8" s="110"/>
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
@@ -19892,7 +19893,7 @@
       <c r="K8" s="18">
         <v>0.44666666666666599</v>
       </c>
-      <c r="P8" s="102"/>
+      <c r="P8" s="110"/>
       <c r="Q8" s="2" t="s">
         <v>6</v>
       </c>
@@ -19915,7 +19916,7 @@
       <c r="X8" s="69"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B9" s="102"/>
+      <c r="B9" s="110"/>
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
@@ -19943,7 +19944,7 @@
       <c r="K9" s="18">
         <v>0.41017800027812501</v>
       </c>
-      <c r="P9" s="102"/>
+      <c r="P9" s="110"/>
       <c r="Q9" s="2" t="s">
         <v>8</v>
       </c>
@@ -19966,7 +19967,7 @@
       <c r="X9" s="69"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B10" s="102"/>
+      <c r="B10" s="110"/>
       <c r="C10" s="22" t="s">
         <v>9</v>
       </c>
@@ -19994,7 +19995,7 @@
       <c r="K10" s="18">
         <v>0.49500251862456501</v>
       </c>
-      <c r="P10" s="102"/>
+      <c r="P10" s="110"/>
       <c r="Q10" s="22" t="s">
         <v>9</v>
       </c>
@@ -20017,7 +20018,7 @@
       <c r="X10" s="69"/>
     </row>
     <row r="11" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="103"/>
+      <c r="B11" s="111"/>
       <c r="C11" s="24" t="s">
         <v>28</v>
       </c>
@@ -20053,7 +20054,7 @@
         <f t="shared" si="0"/>
         <v>0.47192604220699064</v>
       </c>
-      <c r="P11" s="103"/>
+      <c r="P11" s="111"/>
       <c r="Q11" s="24" t="s">
         <v>28</v>
       </c>
@@ -20078,7 +20079,7 @@
       <c r="X11" s="69"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B12" s="101" t="s">
+      <c r="B12" s="109" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -20108,7 +20109,7 @@
       <c r="K12" s="15">
         <v>0.37968877968877901</v>
       </c>
-      <c r="P12" s="101" t="s">
+      <c r="P12" s="109" t="s">
         <v>49</v>
       </c>
       <c r="Q12" s="7" t="s">
@@ -20133,7 +20134,7 @@
       <c r="X12" s="69"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B13" s="102"/>
+      <c r="B13" s="110"/>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
@@ -20161,7 +20162,7 @@
       <c r="K13" s="18">
         <v>0.39484960917629702</v>
       </c>
-      <c r="P13" s="102"/>
+      <c r="P13" s="110"/>
       <c r="Q13" s="2" t="s">
         <v>5</v>
       </c>
@@ -20184,7 +20185,7 @@
       <c r="X13" s="69"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B14" s="102"/>
+      <c r="B14" s="110"/>
       <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
@@ -20212,7 +20213,7 @@
       <c r="K14" s="18">
         <v>0.40748727163821502</v>
       </c>
-      <c r="P14" s="102"/>
+      <c r="P14" s="110"/>
       <c r="Q14" s="2" t="s">
         <v>6</v>
       </c>
@@ -20235,7 +20236,7 @@
       <c r="X14" s="69"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B15" s="102"/>
+      <c r="B15" s="110"/>
       <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
@@ -20263,7 +20264,7 @@
       <c r="K15" s="18">
         <v>0.40951374720683897</v>
       </c>
-      <c r="P15" s="102"/>
+      <c r="P15" s="110"/>
       <c r="Q15" s="2" t="s">
         <v>8</v>
       </c>
@@ -20286,7 +20287,7 @@
       <c r="X15" s="69"/>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B16" s="102"/>
+      <c r="B16" s="110"/>
       <c r="C16" s="22" t="s">
         <v>9</v>
       </c>
@@ -20314,7 +20315,7 @@
       <c r="K16" s="18">
         <v>0.41772262371900498</v>
       </c>
-      <c r="P16" s="102"/>
+      <c r="P16" s="110"/>
       <c r="Q16" s="22" t="s">
         <v>9</v>
       </c>
@@ -20337,7 +20338,7 @@
       <c r="X16" s="69"/>
     </row>
     <row r="17" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="103"/>
+      <c r="B17" s="111"/>
       <c r="C17" s="24" t="s">
         <v>28</v>
       </c>
@@ -20373,7 +20374,7 @@
         <f t="shared" si="1"/>
         <v>0.40185240628582697</v>
       </c>
-      <c r="P17" s="103"/>
+      <c r="P17" s="111"/>
       <c r="Q17" s="24" t="s">
         <v>28</v>
       </c>
@@ -20398,7 +20399,7 @@
       <c r="X17" s="69"/>
     </row>
     <row r="18" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B18" s="101" t="s">
+      <c r="B18" s="109" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -20428,7 +20429,7 @@
       <c r="K18" s="15">
         <v>0.56784646348476098</v>
       </c>
-      <c r="P18" s="101" t="s">
+      <c r="P18" s="109" t="s">
         <v>14</v>
       </c>
       <c r="Q18" s="7" t="s">
@@ -20453,7 +20454,7 @@
       <c r="X18" s="69"/>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B19" s="102"/>
+      <c r="B19" s="110"/>
       <c r="C19" s="2" t="s">
         <v>5</v>
       </c>
@@ -20481,7 +20482,7 @@
       <c r="K19" s="18">
         <v>0.46253496058987997</v>
       </c>
-      <c r="P19" s="102"/>
+      <c r="P19" s="110"/>
       <c r="Q19" s="2" t="s">
         <v>5</v>
       </c>
@@ -20504,7 +20505,7 @@
       <c r="X19" s="69"/>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B20" s="102"/>
+      <c r="B20" s="110"/>
       <c r="C20" s="2" t="s">
         <v>6</v>
       </c>
@@ -20532,7 +20533,7 @@
       <c r="K20" s="18">
         <v>0.50257522316750003</v>
       </c>
-      <c r="P20" s="102"/>
+      <c r="P20" s="110"/>
       <c r="Q20" s="2" t="s">
         <v>6</v>
       </c>
@@ -20555,7 +20556,7 @@
       <c r="X20" s="69"/>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B21" s="102"/>
+      <c r="B21" s="110"/>
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
@@ -20583,7 +20584,7 @@
       <c r="K21" s="18">
         <v>0.49256491545893699</v>
       </c>
-      <c r="P21" s="102"/>
+      <c r="P21" s="110"/>
       <c r="Q21" s="2" t="s">
         <v>8</v>
       </c>
@@ -20606,7 +20607,7 @@
       <c r="X21" s="69"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B22" s="102"/>
+      <c r="B22" s="110"/>
       <c r="C22" s="22" t="s">
         <v>9</v>
       </c>
@@ -20634,7 +20635,7 @@
       <c r="K22" s="18">
         <v>0.53429525850500204</v>
       </c>
-      <c r="P22" s="102"/>
+      <c r="P22" s="110"/>
       <c r="Q22" s="22" t="s">
         <v>9</v>
       </c>
@@ -20657,7 +20658,7 @@
       <c r="X22" s="69"/>
     </row>
     <row r="23" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="103"/>
+      <c r="B23" s="111"/>
       <c r="C23" s="24" t="s">
         <v>28</v>
       </c>
@@ -20693,7 +20694,7 @@
         <f t="shared" si="3"/>
         <v>0.51196336424121602</v>
       </c>
-      <c r="P23" s="103"/>
+      <c r="P23" s="111"/>
       <c r="Q23" s="24" t="s">
         <v>28</v>
       </c>
@@ -20772,7 +20773,7 @@
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="101" t="s">
+      <c r="B37" s="109" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="8" t="s">
@@ -20783,7 +20784,7 @@
       </c>
     </row>
     <row r="38" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="102"/>
+      <c r="B38" s="110"/>
       <c r="C38" s="1" t="s">
         <v>45</v>
       </c>
@@ -20792,7 +20793,7 @@
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="102"/>
+      <c r="B39" s="110"/>
       <c r="C39" s="1" t="s">
         <v>46</v>
       </c>
@@ -20801,7 +20802,7 @@
       </c>
     </row>
     <row r="40" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="103"/>
+      <c r="B40" s="111"/>
       <c r="C40" s="4" t="s">
         <v>47</v>
       </c>
@@ -20810,7 +20811,7 @@
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="101" t="s">
+      <c r="B41" s="109" t="s">
         <v>49</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -20821,7 +20822,7 @@
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="102"/>
+      <c r="B42" s="110"/>
       <c r="C42" s="1" t="s">
         <v>45</v>
       </c>
@@ -20830,7 +20831,7 @@
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="102"/>
+      <c r="B43" s="110"/>
       <c r="C43" s="1" t="s">
         <v>46</v>
       </c>
@@ -20839,7 +20840,7 @@
       </c>
     </row>
     <row r="44" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="103"/>
+      <c r="B44" s="111"/>
       <c r="C44" s="4" t="s">
         <v>47</v>
       </c>
@@ -20848,7 +20849,7 @@
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="101" t="s">
+      <c r="B45" s="109" t="s">
         <v>42</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -20859,7 +20860,7 @@
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="102"/>
+      <c r="B46" s="110"/>
       <c r="C46" s="1" t="s">
         <v>45</v>
       </c>
@@ -20868,7 +20869,7 @@
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="102"/>
+      <c r="B47" s="110"/>
       <c r="C47" s="1" t="s">
         <v>46</v>
       </c>
@@ -20877,7 +20878,7 @@
       </c>
     </row>
     <row r="48" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="103"/>
+      <c r="B48" s="111"/>
       <c r="C48" s="4" t="s">
         <v>47</v>
       </c>
@@ -20902,7 +20903,7 @@
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B53" s="101" t="s">
+      <c r="B53" s="109" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="89" t="s">
@@ -20913,7 +20914,7 @@
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B54" s="102"/>
+      <c r="B54" s="110"/>
       <c r="C54" s="90" t="s">
         <v>45</v>
       </c>
@@ -20922,7 +20923,7 @@
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B55" s="102"/>
+      <c r="B55" s="110"/>
       <c r="C55" s="90" t="s">
         <v>46</v>
       </c>
@@ -20931,7 +20932,7 @@
       </c>
     </row>
     <row r="56" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="103"/>
+      <c r="B56" s="111"/>
       <c r="C56" s="91" t="s">
         <v>47</v>
       </c>
@@ -20940,7 +20941,7 @@
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B57" s="101" t="s">
+      <c r="B57" s="109" t="s">
         <v>49</v>
       </c>
       <c r="C57" s="89" t="s">
@@ -20951,7 +20952,7 @@
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B58" s="102"/>
+      <c r="B58" s="110"/>
       <c r="C58" s="90" t="s">
         <v>45</v>
       </c>
@@ -20960,7 +20961,7 @@
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B59" s="102"/>
+      <c r="B59" s="110"/>
       <c r="C59" s="90" t="s">
         <v>46</v>
       </c>
@@ -20969,7 +20970,7 @@
       </c>
     </row>
     <row r="60" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="103"/>
+      <c r="B60" s="111"/>
       <c r="C60" s="91" t="s">
         <v>47</v>
       </c>
@@ -20978,7 +20979,7 @@
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B61" s="101" t="s">
+      <c r="B61" s="109" t="s">
         <v>42</v>
       </c>
       <c r="C61" s="89" t="s">
@@ -20989,7 +20990,7 @@
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B62" s="102"/>
+      <c r="B62" s="110"/>
       <c r="C62" s="90" t="s">
         <v>45</v>
       </c>
@@ -20998,7 +20999,7 @@
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B63" s="102"/>
+      <c r="B63" s="110"/>
       <c r="C63" s="90" t="s">
         <v>46</v>
       </c>
@@ -21007,7 +21008,7 @@
       </c>
     </row>
     <row r="64" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="103"/>
+      <c r="B64" s="111"/>
       <c r="C64" s="91" t="s">
         <v>47</v>
       </c>
@@ -21017,12 +21018,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="B45:B48"/>
     <mergeCell ref="T4:U4"/>
     <mergeCell ref="R4:S4"/>
     <mergeCell ref="B12:B17"/>
@@ -21039,6 +21034,12 @@
     <mergeCell ref="P6:P11"/>
     <mergeCell ref="P12:P17"/>
     <mergeCell ref="P18:P23"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B45:B48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>